<commit_message>
Changes to object repository
</commit_message>
<xml_diff>
--- a/P002_090_Dispatcher_Config.xlsx
+++ b/P002_090_Dispatcher_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55651C\Documents\UiPath\P002_090_PayCycleAfternoon_Dispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4359CE3-2BAF-4255-869E-6237462DD726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52DEB20-F430-482C-9D5D-081AC854DA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -995,9 +995,6 @@
     <t>MailFilterEndTime</t>
   </si>
   <si>
-    <t>11:30AM</t>
-  </si>
-  <si>
     <t>P002_090_PayCycleAfternoon_PayCycleValues</t>
   </si>
   <si>
@@ -1029,6 +1026,9 @@
   </si>
   <si>
     <t>P002_090_PayCycleAfternoon_Dispatcher</t>
+  </si>
+  <si>
+    <t>11:30PM</t>
   </si>
 </sst>
 </file>
@@ -1580,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -1631,7 +1631,7 @@
         <v>272</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1642,7 +1642,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -1653,7 +1653,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>21</v>
@@ -2258,7 +2258,7 @@
         <v>227</v>
       </c>
       <c r="B63" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2266,7 +2266,7 @@
         <v>228</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2306,7 +2306,7 @@
         <v>314</v>
       </c>
       <c r="B69" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2322,12 +2322,12 @@
         <v>317</v>
       </c>
       <c r="B71" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B72" t="b">
         <v>1</v>
@@ -2335,11 +2335,11 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B73" t="str">
         <f ca="1">TEXT(TODAY(), "mm/dd/yyyy")</f>
-        <v>12/13/2023</v>
+        <v>12/14/2023</v>
       </c>
     </row>
   </sheetData>
@@ -3533,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -3566,10 +3566,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>